<commit_message>
Spectral substraction implementado con exito, buenos resultados aunque un pelin peor que mi percentile algorithm
</commit_message>
<xml_diff>
--- a/Resultados/Resultados_Linkados.xlsx
+++ b/Resultados/Resultados_Linkados.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="23">
   <si>
     <t xml:space="preserve">2nd Event:    </t>
   </si>
@@ -85,6 +85,9 @@
   </si>
   <si>
     <t>SAME AS WITHOUT FILTER</t>
+  </si>
+  <si>
+    <t>Spectral substraction</t>
   </si>
 </sst>
 </file>
@@ -123,7 +126,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -166,6 +169,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="15">
     <border>
@@ -345,7 +354,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -378,7 +387,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -391,7 +399,6 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -412,6 +419,9 @@
     </xf>
     <xf numFmtId="1" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="2" fontId="1" fillId="7" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -425,7 +435,10 @@
     <xf numFmtId="2" fontId="1" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -446,9 +459,6 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -464,13 +474,19 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -767,10 +783,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J61"/>
+  <dimension ref="A1:J68"/>
   <sheetViews>
-    <sheetView tabSelected="1" showWhiteSpace="0" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="D38" sqref="D38"/>
+    <sheetView tabSelected="1" showWhiteSpace="0" topLeftCell="A50" workbookViewId="0">
+      <selection activeCell="I68" sqref="I68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -785,33 +801,33 @@
       <c r="A1" s="37" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="42" t="s">
+      <c r="B1" s="41" t="s">
         <v>9</v>
       </c>
-      <c r="C1" s="42"/>
-      <c r="D1" s="42"/>
-      <c r="E1" s="42"/>
-      <c r="F1" s="43" t="s">
+      <c r="C1" s="41"/>
+      <c r="D1" s="41"/>
+      <c r="E1" s="41"/>
+      <c r="F1" s="42" t="s">
         <v>10</v>
       </c>
-      <c r="G1" s="42"/>
-      <c r="H1" s="42"/>
-      <c r="I1" s="44"/>
+      <c r="G1" s="41"/>
+      <c r="H1" s="41"/>
+      <c r="I1" s="43"/>
     </row>
     <row r="2" spans="1:10" ht="15.75" thickBot="1">
       <c r="A2" s="38"/>
-      <c r="B2" s="41" t="s">
+      <c r="B2" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="41"/>
-      <c r="D2" s="41" t="s">
+      <c r="C2" s="40"/>
+      <c r="D2" s="40" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="41"/>
+      <c r="E2" s="40"/>
       <c r="F2" s="34" t="s">
         <v>11</v>
       </c>
-      <c r="G2" s="45"/>
+      <c r="G2" s="44"/>
       <c r="H2" s="34" t="s">
         <v>12</v>
       </c>
@@ -868,34 +884,34 @@
       <c r="I5" s="36"/>
     </row>
     <row r="6" spans="1:10">
-      <c r="A6" s="40"/>
-      <c r="B6" s="40"/>
-      <c r="C6" s="40"/>
-      <c r="D6" s="40"/>
-      <c r="E6" s="40"/>
-      <c r="F6" s="40"/>
-      <c r="G6" s="40"/>
-      <c r="H6" s="40"/>
-      <c r="I6" s="40"/>
+      <c r="A6" s="33"/>
+      <c r="B6" s="33"/>
+      <c r="C6" s="33"/>
+      <c r="D6" s="33"/>
+      <c r="E6" s="33"/>
+      <c r="F6" s="33"/>
+      <c r="G6" s="33"/>
+      <c r="H6" s="33"/>
+      <c r="I6" s="33"/>
     </row>
     <row r="7" spans="1:10" ht="15.75">
       <c r="A7" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="B7" s="33" t="s">
+      <c r="B7" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="C7" s="33"/>
+      <c r="C7" s="27"/>
       <c r="D7" s="14"/>
-      <c r="E7" s="33" t="s">
+      <c r="E7" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="F7" s="33"/>
+      <c r="F7" s="27"/>
       <c r="G7" s="14"/>
-      <c r="H7" s="33" t="s">
+      <c r="H7" s="27" t="s">
         <v>3</v>
       </c>
-      <c r="I7" s="33"/>
+      <c r="I7" s="27"/>
     </row>
     <row r="8" spans="1:10" ht="15.75">
       <c r="A8" s="12"/>
@@ -924,95 +940,95 @@
       <c r="A9" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="B9" s="23">
+      <c r="B9" s="21">
         <f>(3.884-B$3)*100/B$3</f>
         <v>1.277705345501954</v>
       </c>
-      <c r="C9" s="24">
+      <c r="C9" s="22">
         <f>372866-C$3</f>
         <v>4706</v>
       </c>
-      <c r="D9" s="22"/>
-      <c r="E9" s="23">
+      <c r="D9" s="20"/>
+      <c r="E9" s="21">
         <f>(3.8395-B$3)*100/B$3</f>
         <v>0.1173402868318167</v>
       </c>
-      <c r="F9" s="24">
+      <c r="F9" s="22">
         <f>368600-C$3</f>
         <v>440</v>
       </c>
-      <c r="G9" s="22"/>
-      <c r="H9" s="23">
+      <c r="G9" s="20"/>
+      <c r="H9" s="21">
         <f>(3.7711-B$3)*100/B$3</f>
         <v>-1.6662320730117299</v>
       </c>
-      <c r="I9" s="24">
+      <c r="I9" s="22">
         <f>362029-C$3</f>
         <v>-6131</v>
       </c>
-      <c r="J9" s="19"/>
+      <c r="J9" s="18"/>
     </row>
     <row r="10" spans="1:10" ht="15.75">
       <c r="A10" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B10" s="23">
+      <c r="B10" s="21">
         <f>(8.902-D$3)*100/D$3</f>
         <v>127.55623721881389</v>
       </c>
-      <c r="C10" s="24">
+      <c r="C10" s="22">
         <f>854685-E$3</f>
         <v>479133</v>
       </c>
-      <c r="D10" s="22"/>
-      <c r="E10" s="23">
+      <c r="D10" s="20"/>
+      <c r="E10" s="21">
         <f>(8.916-D$3)*100/D$3</f>
         <v>127.91411042944786</v>
       </c>
-      <c r="F10" s="24">
+      <c r="F10" s="22">
         <f>856019-E$3</f>
         <v>480467</v>
       </c>
-      <c r="G10" s="22"/>
-      <c r="H10" s="23">
+      <c r="G10" s="20"/>
+      <c r="H10" s="21">
         <f>(8.108-D$3)*100/D$3</f>
         <v>107.25971370143152</v>
       </c>
-      <c r="I10" s="24">
+      <c r="I10" s="22">
         <f>778456-E$3</f>
         <v>402904</v>
       </c>
-      <c r="J10" s="19"/>
+      <c r="J10" s="18"/>
     </row>
     <row r="11" spans="1:10">
       <c r="A11" s="3"/>
-      <c r="B11" s="17"/>
-      <c r="C11" s="19"/>
-      <c r="D11" s="18"/>
-      <c r="E11" s="18"/>
-      <c r="F11" s="19"/>
-      <c r="G11" s="17"/>
-      <c r="H11" s="18"/>
-      <c r="I11" s="18"/>
+      <c r="B11" s="16"/>
+      <c r="C11" s="18"/>
+      <c r="D11" s="17"/>
+      <c r="E11" s="17"/>
+      <c r="F11" s="18"/>
+      <c r="G11" s="16"/>
+      <c r="H11" s="17"/>
+      <c r="I11" s="17"/>
     </row>
     <row r="12" spans="1:10" ht="15.75">
       <c r="A12" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="B12" s="33" t="s">
+      <c r="B12" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="C12" s="33"/>
+      <c r="C12" s="27"/>
       <c r="D12" s="14"/>
-      <c r="E12" s="33" t="s">
+      <c r="E12" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="F12" s="33"/>
+      <c r="F12" s="27"/>
       <c r="G12" s="14"/>
-      <c r="H12" s="33" t="s">
+      <c r="H12" s="27" t="s">
         <v>3</v>
       </c>
-      <c r="I12" s="33"/>
+      <c r="I12" s="27"/>
     </row>
     <row r="13" spans="1:10" ht="15.75">
       <c r="A13" s="12"/>
@@ -1041,29 +1057,29 @@
       <c r="A14" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="B14" s="23">
+      <c r="B14" s="21">
         <f>(5.618-F$3)*100/F$3</f>
         <v>0.97052480230050808</v>
       </c>
-      <c r="C14" s="24">
+      <c r="C14" s="22">
         <f>539331-G$3</f>
         <v>5187</v>
       </c>
-      <c r="D14" s="22"/>
-      <c r="E14" s="23">
+      <c r="D14" s="20"/>
+      <c r="E14" s="21">
         <f>(5.618-F$3)*100/F$3</f>
         <v>0.97052480230050808</v>
       </c>
-      <c r="F14" s="24">
+      <c r="F14" s="22">
         <f>539331-G$3</f>
         <v>5187</v>
       </c>
-      <c r="G14" s="22"/>
-      <c r="H14" s="23">
+      <c r="G14" s="20"/>
+      <c r="H14" s="21">
         <f>(5.241-F$3)*100/F$3</f>
         <v>-5.8051761322789428</v>
       </c>
-      <c r="I14" s="24">
+      <c r="I14" s="22">
         <f>503412-G$3</f>
         <v>-30732</v>
       </c>
@@ -1072,95 +1088,95 @@
       <c r="A15" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B15" s="23">
+      <c r="B15" s="21">
         <f>(10.76-H$3)*100/H$3</f>
         <v>86.094776893808358</v>
       </c>
-      <c r="C15" s="24">
+      <c r="C15" s="22">
         <f>1033350-I$3</f>
         <v>478278</v>
       </c>
-      <c r="D15" s="22"/>
-      <c r="E15" s="23">
+      <c r="D15" s="20"/>
+      <c r="E15" s="21">
         <f>(10.601-H$3)*100/H$3</f>
         <v>83.344863369076464</v>
       </c>
-      <c r="F15" s="24">
+      <c r="F15" s="22">
         <f>1017704-I$3</f>
         <v>462632</v>
       </c>
-      <c r="G15" s="22"/>
-      <c r="H15" s="23">
+      <c r="G15" s="20"/>
+      <c r="H15" s="21">
         <f>(10.77-H$3)*100/H$3</f>
         <v>86.267727429955031</v>
       </c>
-      <c r="I15" s="24">
+      <c r="I15" s="22">
         <f>1034272-I$3</f>
         <v>479200</v>
       </c>
     </row>
     <row r="16" spans="1:10">
-      <c r="B16" s="17"/>
-      <c r="C16" s="19"/>
-      <c r="D16" s="18"/>
-      <c r="E16" s="18"/>
-      <c r="F16" s="20"/>
-      <c r="G16" s="18"/>
-      <c r="H16" s="18"/>
-      <c r="I16" s="18"/>
+      <c r="B16" s="16"/>
+      <c r="C16" s="18"/>
+      <c r="D16" s="17"/>
+      <c r="E16" s="17"/>
+      <c r="F16" s="19"/>
+      <c r="G16" s="17"/>
+      <c r="H16" s="17"/>
+      <c r="I16" s="17"/>
     </row>
     <row r="17" spans="1:9">
-      <c r="B17" s="17"/>
-      <c r="C17" s="19"/>
-      <c r="D17" s="18"/>
-      <c r="E17" s="18"/>
-      <c r="F17" s="20"/>
-      <c r="G17" s="18"/>
-      <c r="H17" s="18"/>
-      <c r="I17" s="18"/>
+      <c r="B17" s="16"/>
+      <c r="C17" s="18"/>
+      <c r="D17" s="17"/>
+      <c r="E17" s="17"/>
+      <c r="F17" s="19"/>
+      <c r="G17" s="17"/>
+      <c r="H17" s="17"/>
+      <c r="I17" s="17"/>
     </row>
     <row r="18" spans="1:9">
-      <c r="A18" s="46" t="s">
+      <c r="A18" s="32" t="s">
         <v>18</v>
       </c>
-      <c r="B18" s="46"/>
-      <c r="C18" s="46"/>
-      <c r="D18" s="46"/>
-      <c r="E18" s="46"/>
-      <c r="F18" s="46"/>
-      <c r="G18" s="46"/>
-      <c r="H18" s="46"/>
-      <c r="I18" s="46"/>
+      <c r="B18" s="32"/>
+      <c r="C18" s="32"/>
+      <c r="D18" s="32"/>
+      <c r="E18" s="32"/>
+      <c r="F18" s="32"/>
+      <c r="G18" s="32"/>
+      <c r="H18" s="32"/>
+      <c r="I18" s="32"/>
     </row>
     <row r="19" spans="1:9">
-      <c r="A19" s="40"/>
-      <c r="B19" s="40"/>
-      <c r="C19" s="40"/>
-      <c r="D19" s="40"/>
-      <c r="E19" s="40"/>
-      <c r="F19" s="40"/>
-      <c r="G19" s="40"/>
-      <c r="H19" s="40"/>
-      <c r="I19" s="40"/>
+      <c r="A19" s="33"/>
+      <c r="B19" s="33"/>
+      <c r="C19" s="33"/>
+      <c r="D19" s="33"/>
+      <c r="E19" s="33"/>
+      <c r="F19" s="33"/>
+      <c r="G19" s="33"/>
+      <c r="H19" s="33"/>
+      <c r="I19" s="33"/>
     </row>
     <row r="20" spans="1:9" ht="15.75">
       <c r="A20" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="B20" s="33" t="s">
+      <c r="B20" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="C20" s="33"/>
+      <c r="C20" s="27"/>
       <c r="D20" s="14"/>
-      <c r="E20" s="33" t="s">
+      <c r="E20" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="F20" s="33"/>
+      <c r="F20" s="27"/>
       <c r="G20" s="14"/>
-      <c r="H20" s="33" t="s">
+      <c r="H20" s="27" t="s">
         <v>3</v>
       </c>
-      <c r="I20" s="33"/>
+      <c r="I20" s="27"/>
     </row>
     <row r="21" spans="1:9" ht="15.75">
       <c r="A21" s="12"/>
@@ -1189,23 +1205,23 @@
       <c r="A22" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="B22" s="27">
+      <c r="B22" s="25">
         <f>(3.8745-B$3)*100/B$3</f>
         <v>1.0299869621903486</v>
       </c>
-      <c r="C22" s="28">
+      <c r="C22" s="26">
         <f>371957-C$3</f>
         <v>3797</v>
       </c>
-      <c r="D22" s="22"/>
-      <c r="E22" s="27"/>
-      <c r="F22" s="28"/>
-      <c r="G22" s="22"/>
-      <c r="H22" s="27">
+      <c r="D22" s="20"/>
+      <c r="E22" s="25"/>
+      <c r="F22" s="26"/>
+      <c r="G22" s="20"/>
+      <c r="H22" s="25">
         <f>(3.8745-B$3)*100/B$3</f>
         <v>1.0299869621903486</v>
       </c>
-      <c r="I22" s="28">
+      <c r="I22" s="26">
         <f>371957-C$3</f>
         <v>3797</v>
       </c>
@@ -1214,56 +1230,56 @@
       <c r="A23" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B23" s="27">
+      <c r="B23" s="25">
         <f>(4-D$3)*100/D$3</f>
         <v>2.2494887525562395</v>
       </c>
-      <c r="C23" s="28">
+      <c r="C23" s="26">
         <f>383698-E$3</f>
         <v>8146</v>
       </c>
-      <c r="D23" s="22"/>
-      <c r="E23" s="27"/>
-      <c r="F23" s="28"/>
-      <c r="G23" s="22"/>
-      <c r="H23" s="27">
+      <c r="D23" s="20"/>
+      <c r="E23" s="25"/>
+      <c r="F23" s="26"/>
+      <c r="G23" s="20"/>
+      <c r="H23" s="25">
         <f>(3.989-D$3)*100/D$3</f>
         <v>1.9683026584867065</v>
       </c>
-      <c r="I23" s="28">
+      <c r="I23" s="26">
         <f>383002-E$3</f>
         <v>7450</v>
       </c>
     </row>
     <row r="24" spans="1:9">
       <c r="A24" s="3"/>
-      <c r="B24" s="17"/>
-      <c r="C24" s="19"/>
-      <c r="D24" s="18"/>
-      <c r="E24" s="18"/>
-      <c r="F24" s="19"/>
-      <c r="G24" s="17"/>
-      <c r="H24" s="18"/>
-      <c r="I24" s="18"/>
+      <c r="B24" s="16"/>
+      <c r="C24" s="18"/>
+      <c r="D24" s="17"/>
+      <c r="E24" s="17"/>
+      <c r="F24" s="18"/>
+      <c r="G24" s="16"/>
+      <c r="H24" s="17"/>
+      <c r="I24" s="17"/>
     </row>
     <row r="25" spans="1:9" ht="15.75">
       <c r="A25" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="B25" s="33" t="s">
+      <c r="B25" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="C25" s="33"/>
+      <c r="C25" s="27"/>
       <c r="D25" s="14"/>
-      <c r="E25" s="33" t="s">
+      <c r="E25" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="F25" s="33"/>
+      <c r="F25" s="27"/>
       <c r="G25" s="14"/>
-      <c r="H25" s="33" t="s">
+      <c r="H25" s="27" t="s">
         <v>3</v>
       </c>
-      <c r="I25" s="33"/>
+      <c r="I25" s="27"/>
     </row>
     <row r="26" spans="1:9" ht="15.75">
       <c r="A26" s="12"/>
@@ -1292,23 +1308,23 @@
       <c r="A27" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="B27" s="27">
+      <c r="B27" s="25">
         <f>(5.574-F$3)*100/F$3</f>
         <v>0.17972681524083009</v>
       </c>
-      <c r="C27" s="28">
+      <c r="C27" s="26">
         <f>535141-G$3</f>
         <v>997</v>
       </c>
-      <c r="D27" s="22"/>
-      <c r="E27" s="27"/>
-      <c r="F27" s="28"/>
-      <c r="G27" s="22"/>
-      <c r="H27" s="27">
+      <c r="D27" s="20"/>
+      <c r="E27" s="25"/>
+      <c r="F27" s="26"/>
+      <c r="G27" s="20"/>
+      <c r="H27" s="25">
         <f>(5.548-F$3)*100/F$3</f>
         <v>-0.28756290438533455</v>
       </c>
-      <c r="I27" s="28">
+      <c r="I27" s="26">
         <f>532634-G$3</f>
         <v>-1510</v>
       </c>
@@ -1317,95 +1333,95 @@
       <c r="A28" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B28" s="27">
+      <c r="B28" s="25">
         <f>(4.999-H$3)*100/H$3</f>
         <v>-13.542026980283646</v>
       </c>
-      <c r="C28" s="28">
+      <c r="C28" s="26">
         <f>479999-I$3</f>
         <v>-75073</v>
       </c>
-      <c r="D28" s="22"/>
-      <c r="E28" s="27">
+      <c r="D28" s="20"/>
+      <c r="E28" s="25">
         <f>(4.999-H$3)*100/H$3</f>
         <v>-13.542026980283646</v>
       </c>
-      <c r="F28" s="28">
+      <c r="F28" s="26">
         <f>479999-I$3</f>
         <v>-75073</v>
       </c>
-      <c r="G28" s="22"/>
-      <c r="H28" s="27">
+      <c r="G28" s="20"/>
+      <c r="H28" s="25">
         <f>(10.866-H$3)*100/H$3</f>
         <v>87.928052576962983</v>
       </c>
-      <c r="I28" s="28">
+      <c r="I28" s="26">
         <f>1043223-I$3</f>
         <v>488151</v>
       </c>
     </row>
     <row r="29" spans="1:9">
-      <c r="B29" s="17"/>
-      <c r="C29" s="19"/>
-      <c r="D29" s="18"/>
-      <c r="E29" s="18"/>
-      <c r="F29" s="20"/>
-      <c r="G29" s="18"/>
-      <c r="H29" s="18"/>
-      <c r="I29" s="18"/>
+      <c r="B29" s="16"/>
+      <c r="C29" s="18"/>
+      <c r="D29" s="17"/>
+      <c r="E29" s="17"/>
+      <c r="F29" s="19"/>
+      <c r="G29" s="17"/>
+      <c r="H29" s="17"/>
+      <c r="I29" s="17"/>
     </row>
     <row r="30" spans="1:9">
-      <c r="B30" s="17"/>
-      <c r="C30" s="19"/>
-      <c r="D30" s="18"/>
-      <c r="E30" s="18"/>
-      <c r="F30" s="20"/>
-      <c r="G30" s="18"/>
-      <c r="H30" s="18"/>
-      <c r="I30" s="18"/>
+      <c r="B30" s="16"/>
+      <c r="C30" s="18"/>
+      <c r="D30" s="17"/>
+      <c r="E30" s="17"/>
+      <c r="F30" s="19"/>
+      <c r="G30" s="17"/>
+      <c r="H30" s="17"/>
+      <c r="I30" s="17"/>
     </row>
     <row r="31" spans="1:9">
-      <c r="A31" s="47" t="s">
+      <c r="A31" s="45" t="s">
         <v>20</v>
       </c>
-      <c r="B31" s="47"/>
-      <c r="C31" s="47"/>
-      <c r="D31" s="47"/>
-      <c r="E31" s="47"/>
-      <c r="F31" s="47"/>
-      <c r="G31" s="47"/>
-      <c r="H31" s="47"/>
-      <c r="I31" s="47"/>
+      <c r="B31" s="45"/>
+      <c r="C31" s="45"/>
+      <c r="D31" s="45"/>
+      <c r="E31" s="45"/>
+      <c r="F31" s="45"/>
+      <c r="G31" s="45"/>
+      <c r="H31" s="45"/>
+      <c r="I31" s="45"/>
     </row>
     <row r="32" spans="1:9">
-      <c r="A32" s="40"/>
-      <c r="B32" s="40"/>
-      <c r="C32" s="40"/>
-      <c r="D32" s="40"/>
-      <c r="E32" s="40"/>
-      <c r="F32" s="40"/>
-      <c r="G32" s="40"/>
-      <c r="H32" s="40"/>
-      <c r="I32" s="40"/>
+      <c r="A32" s="33"/>
+      <c r="B32" s="33"/>
+      <c r="C32" s="33"/>
+      <c r="D32" s="33"/>
+      <c r="E32" s="33"/>
+      <c r="F32" s="33"/>
+      <c r="G32" s="33"/>
+      <c r="H32" s="33"/>
+      <c r="I32" s="33"/>
     </row>
     <row r="33" spans="1:9" ht="15.75">
       <c r="A33" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="B33" s="33" t="s">
+      <c r="B33" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="C33" s="33"/>
+      <c r="C33" s="27"/>
       <c r="D33" s="14"/>
-      <c r="E33" s="33" t="s">
+      <c r="E33" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="F33" s="33"/>
+      <c r="F33" s="27"/>
       <c r="G33" s="14"/>
-      <c r="H33" s="33" t="s">
+      <c r="H33" s="27" t="s">
         <v>3</v>
       </c>
-      <c r="I33" s="33"/>
+      <c r="I33" s="27"/>
     </row>
     <row r="34" spans="1:9" ht="15.75">
       <c r="A34" s="12"/>
@@ -1434,29 +1450,29 @@
       <c r="A35" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="B35" s="25">
+      <c r="B35" s="23">
         <f>((367200/96000)-B$3)*100/B$3</f>
         <v>-0.26075619295957725</v>
       </c>
-      <c r="C35" s="26">
+      <c r="C35" s="24">
         <f>367200-C$3</f>
         <v>-960</v>
       </c>
-      <c r="D35" s="22"/>
-      <c r="E35" s="25">
+      <c r="D35" s="20"/>
+      <c r="E35" s="23">
         <f>((374330/96000)-B$3)*100/B$3</f>
         <v>1.6759017818339896</v>
       </c>
-      <c r="F35" s="26">
+      <c r="F35" s="24">
         <f>374330-C$3</f>
         <v>6170</v>
       </c>
-      <c r="G35" s="22"/>
-      <c r="H35" s="25">
+      <c r="G35" s="20"/>
+      <c r="H35" s="23">
         <f>(3.825-B$3)*100/B$3</f>
         <v>-0.26075619295957725</v>
       </c>
-      <c r="I35" s="26">
+      <c r="I35" s="24">
         <f>367200-C$3</f>
         <v>-960</v>
       </c>
@@ -1465,62 +1481,62 @@
       <c r="A36" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B36" s="25">
+      <c r="B36" s="23">
         <f>((374400/96000)-D$3)*100/D$3</f>
         <v>-0.30674846625766899</v>
       </c>
-      <c r="C36" s="26">
+      <c r="C36" s="24">
         <f>374400 -E$3</f>
         <v>-1152</v>
       </c>
-      <c r="D36" s="22"/>
-      <c r="E36" s="25">
+      <c r="D36" s="20"/>
+      <c r="E36" s="23">
         <f>((370800/96000)-D$3)*100/D$3</f>
         <v>-1.265337423312886</v>
       </c>
-      <c r="F36" s="26">
+      <c r="F36" s="24">
         <f>370800-E$3</f>
         <v>-4752</v>
       </c>
-      <c r="G36" s="22"/>
-      <c r="H36" s="25">
+      <c r="G36" s="20"/>
+      <c r="H36" s="23">
         <f>((378000/96000)-D$3)*100/D$3</f>
         <v>0.65184049079754802</v>
       </c>
-      <c r="I36" s="26">
+      <c r="I36" s="24">
         <f>378000-E$3</f>
         <v>2448</v>
       </c>
     </row>
     <row r="37" spans="1:9">
       <c r="A37" s="3"/>
-      <c r="B37" s="17"/>
-      <c r="C37" s="19"/>
-      <c r="D37" s="18"/>
-      <c r="E37" s="18"/>
-      <c r="F37" s="19"/>
-      <c r="G37" s="17"/>
-      <c r="H37" s="18"/>
-      <c r="I37" s="18"/>
+      <c r="B37" s="16"/>
+      <c r="C37" s="18"/>
+      <c r="D37" s="17"/>
+      <c r="E37" s="17"/>
+      <c r="F37" s="18"/>
+      <c r="G37" s="16"/>
+      <c r="H37" s="17"/>
+      <c r="I37" s="17"/>
     </row>
     <row r="38" spans="1:9" ht="15.75">
       <c r="A38" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="B38" s="33" t="s">
+      <c r="B38" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="C38" s="33"/>
+      <c r="C38" s="27"/>
       <c r="D38" s="14"/>
-      <c r="E38" s="33" t="s">
+      <c r="E38" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="F38" s="33"/>
+      <c r="F38" s="27"/>
       <c r="G38" s="14"/>
-      <c r="H38" s="33" t="s">
+      <c r="H38" s="27" t="s">
         <v>3</v>
       </c>
-      <c r="I38" s="33"/>
+      <c r="I38" s="27"/>
     </row>
     <row r="39" spans="1:9" ht="15.75">
       <c r="A39" s="12"/>
@@ -1549,29 +1565,29 @@
       <c r="A40" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="B40" s="25">
+      <c r="B40" s="23">
         <f>((532800/96000)-F$3)*100/F$3</f>
         <v>-0.25161754133717174</v>
       </c>
-      <c r="C40" s="26">
+      <c r="C40" s="24">
         <f>532800-G$3</f>
         <v>-1344</v>
       </c>
-      <c r="D40" s="22"/>
-      <c r="E40" s="25">
+      <c r="D40" s="20"/>
+      <c r="E40" s="23">
         <f>((532730/96000)-F$3)*100/F$3</f>
         <v>-0.26472262161515325</v>
       </c>
-      <c r="F40" s="26">
+      <c r="F40" s="24">
         <f>532730-G$3</f>
         <v>-1414</v>
       </c>
-      <c r="G40" s="22"/>
-      <c r="H40" s="25">
+      <c r="G40" s="20"/>
+      <c r="H40" s="23">
         <f>((532800/96000)-F$3)*100/F$3</f>
         <v>-0.25161754133717174</v>
       </c>
-      <c r="I40" s="26">
+      <c r="I40" s="24">
         <f>532800-G$3</f>
         <v>-1344</v>
       </c>
@@ -1580,95 +1596,95 @@
       <c r="A41" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B41" s="25">
+      <c r="B41" s="23">
         <f>((554400/96000)-H$3)*100/H$3</f>
         <v>-0.12106537530265779</v>
       </c>
-      <c r="C41" s="26">
+      <c r="C41" s="24">
         <f>554400-I$3</f>
         <v>-672</v>
       </c>
-      <c r="D41" s="22"/>
-      <c r="E41" s="25">
+      <c r="D41" s="20"/>
+      <c r="E41" s="23">
         <f>((554401/96000)-H$3)*100/H$3</f>
         <v>-0.12088521849418106</v>
       </c>
-      <c r="F41" s="26">
+      <c r="F41" s="24">
         <f>554401-I$3</f>
         <v>-671</v>
       </c>
-      <c r="G41" s="22"/>
-      <c r="H41" s="25">
+      <c r="G41" s="20"/>
+      <c r="H41" s="23">
         <f>((554401/96000)-H$3)*100/H$3</f>
         <v>-0.12088521849418106</v>
       </c>
-      <c r="I41" s="26">
+      <c r="I41" s="24">
         <f>554401-I$3</f>
         <v>-671</v>
       </c>
     </row>
     <row r="42" spans="1:9">
-      <c r="B42" s="17"/>
-      <c r="C42" s="19"/>
-      <c r="D42" s="18"/>
-      <c r="E42" s="18"/>
-      <c r="F42" s="20"/>
-      <c r="G42" s="18"/>
-      <c r="H42" s="18"/>
-      <c r="I42" s="18"/>
+      <c r="B42" s="16"/>
+      <c r="C42" s="18"/>
+      <c r="D42" s="17"/>
+      <c r="E42" s="17"/>
+      <c r="F42" s="19"/>
+      <c r="G42" s="17"/>
+      <c r="H42" s="17"/>
+      <c r="I42" s="17"/>
     </row>
     <row r="43" spans="1:9">
-      <c r="B43" s="17"/>
-      <c r="C43" s="19"/>
-      <c r="D43" s="18"/>
-      <c r="E43" s="18"/>
-      <c r="F43" s="20"/>
-      <c r="G43" s="18"/>
-      <c r="H43" s="18"/>
-      <c r="I43" s="18"/>
+      <c r="B43" s="16"/>
+      <c r="C43" s="18"/>
+      <c r="D43" s="17"/>
+      <c r="E43" s="17"/>
+      <c r="F43" s="19"/>
+      <c r="G43" s="17"/>
+      <c r="H43" s="17"/>
+      <c r="I43" s="17"/>
     </row>
     <row r="44" spans="1:9">
-      <c r="A44" s="48" t="s">
+      <c r="A44" s="46" t="s">
         <v>19</v>
       </c>
-      <c r="B44" s="48"/>
-      <c r="C44" s="48"/>
-      <c r="D44" s="48"/>
-      <c r="E44" s="48"/>
-      <c r="F44" s="48"/>
-      <c r="G44" s="48"/>
-      <c r="H44" s="48"/>
-      <c r="I44" s="48"/>
+      <c r="B44" s="46"/>
+      <c r="C44" s="46"/>
+      <c r="D44" s="46"/>
+      <c r="E44" s="46"/>
+      <c r="F44" s="46"/>
+      <c r="G44" s="46"/>
+      <c r="H44" s="46"/>
+      <c r="I44" s="46"/>
     </row>
     <row r="45" spans="1:9">
-      <c r="A45" s="40"/>
-      <c r="B45" s="40"/>
-      <c r="C45" s="40"/>
-      <c r="D45" s="40"/>
-      <c r="E45" s="40"/>
-      <c r="F45" s="40"/>
-      <c r="G45" s="40"/>
-      <c r="H45" s="40"/>
-      <c r="I45" s="40"/>
+      <c r="A45" s="33"/>
+      <c r="B45" s="33"/>
+      <c r="C45" s="33"/>
+      <c r="D45" s="33"/>
+      <c r="E45" s="33"/>
+      <c r="F45" s="33"/>
+      <c r="G45" s="33"/>
+      <c r="H45" s="33"/>
+      <c r="I45" s="33"/>
     </row>
     <row r="46" spans="1:9" ht="15.75">
       <c r="A46" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="B46" s="33" t="s">
+      <c r="B46" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="C46" s="33"/>
+      <c r="C46" s="27"/>
       <c r="D46" s="14"/>
-      <c r="E46" s="33" t="s">
+      <c r="E46" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="F46" s="33"/>
+      <c r="F46" s="27"/>
       <c r="G46" s="14"/>
-      <c r="H46" s="33" t="s">
+      <c r="H46" s="27" t="s">
         <v>3</v>
       </c>
-      <c r="I46" s="33"/>
+      <c r="I46" s="27"/>
     </row>
     <row r="47" spans="1:9" ht="15.75">
       <c r="A47" s="12"/>
@@ -1697,63 +1713,63 @@
       <c r="A48" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="B48" s="29" t="s">
+      <c r="B48" s="28" t="s">
         <v>21</v>
       </c>
-      <c r="C48" s="30"/>
-      <c r="D48" s="22"/>
-      <c r="E48" s="29" t="s">
+      <c r="C48" s="29"/>
+      <c r="D48" s="20"/>
+      <c r="E48" s="28" t="s">
         <v>21</v>
       </c>
-      <c r="F48" s="30"/>
-      <c r="G48" s="22"/>
-      <c r="H48" s="29" t="s">
+      <c r="F48" s="29"/>
+      <c r="G48" s="20"/>
+      <c r="H48" s="28" t="s">
         <v>21</v>
       </c>
-      <c r="I48" s="30"/>
+      <c r="I48" s="29"/>
     </row>
     <row r="49" spans="1:9" ht="15.75">
       <c r="A49" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B49" s="31"/>
-      <c r="C49" s="32"/>
-      <c r="D49" s="22"/>
-      <c r="E49" s="31"/>
-      <c r="F49" s="32"/>
-      <c r="G49" s="22"/>
-      <c r="H49" s="31"/>
-      <c r="I49" s="32"/>
+      <c r="B49" s="30"/>
+      <c r="C49" s="31"/>
+      <c r="D49" s="20"/>
+      <c r="E49" s="30"/>
+      <c r="F49" s="31"/>
+      <c r="G49" s="20"/>
+      <c r="H49" s="30"/>
+      <c r="I49" s="31"/>
     </row>
     <row r="50" spans="1:9">
       <c r="A50" s="3"/>
-      <c r="B50" s="17"/>
-      <c r="C50" s="19"/>
-      <c r="D50" s="18"/>
-      <c r="E50" s="18"/>
-      <c r="F50" s="19"/>
-      <c r="G50" s="17"/>
-      <c r="H50" s="18"/>
-      <c r="I50" s="18"/>
+      <c r="B50" s="16"/>
+      <c r="C50" s="18"/>
+      <c r="D50" s="17"/>
+      <c r="E50" s="17"/>
+      <c r="F50" s="18"/>
+      <c r="G50" s="16"/>
+      <c r="H50" s="17"/>
+      <c r="I50" s="17"/>
     </row>
     <row r="51" spans="1:9" ht="15.75">
       <c r="A51" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="B51" s="33" t="s">
+      <c r="B51" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="C51" s="33"/>
+      <c r="C51" s="27"/>
       <c r="D51" s="14"/>
-      <c r="E51" s="33" t="s">
+      <c r="E51" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="F51" s="33"/>
+      <c r="F51" s="27"/>
       <c r="G51" s="14"/>
-      <c r="H51" s="33" t="s">
+      <c r="H51" s="27" t="s">
         <v>3</v>
       </c>
-      <c r="I51" s="33"/>
+      <c r="I51" s="27"/>
     </row>
     <row r="52" spans="1:9" ht="15.75">
       <c r="A52" s="12"/>
@@ -1782,135 +1798,317 @@
       <c r="A53" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="B53" s="29" t="s">
+      <c r="B53" s="28" t="s">
         <v>21</v>
       </c>
-      <c r="C53" s="30"/>
-      <c r="D53" s="22"/>
-      <c r="E53" s="29" t="s">
+      <c r="C53" s="29"/>
+      <c r="D53" s="20"/>
+      <c r="E53" s="28" t="s">
         <v>21</v>
       </c>
-      <c r="F53" s="30"/>
-      <c r="G53" s="22"/>
-      <c r="H53" s="29" t="s">
+      <c r="F53" s="29"/>
+      <c r="G53" s="20"/>
+      <c r="H53" s="28" t="s">
         <v>21</v>
       </c>
-      <c r="I53" s="30"/>
+      <c r="I53" s="29"/>
     </row>
     <row r="54" spans="1:9" ht="15.75">
       <c r="A54" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B54" s="31"/>
-      <c r="C54" s="32"/>
-      <c r="D54" s="22"/>
-      <c r="E54" s="31"/>
-      <c r="F54" s="32"/>
-      <c r="G54" s="22"/>
-      <c r="H54" s="31"/>
-      <c r="I54" s="32"/>
+      <c r="B54" s="30"/>
+      <c r="C54" s="31"/>
+      <c r="D54" s="20"/>
+      <c r="E54" s="30"/>
+      <c r="F54" s="31"/>
+      <c r="G54" s="20"/>
+      <c r="H54" s="30"/>
+      <c r="I54" s="31"/>
     </row>
     <row r="55" spans="1:9">
-      <c r="B55" s="18"/>
-      <c r="C55" s="20"/>
-      <c r="D55" s="18"/>
-      <c r="E55" s="18"/>
-      <c r="F55" s="18"/>
-      <c r="G55" s="18"/>
-      <c r="H55" s="18"/>
-      <c r="I55" s="18"/>
+      <c r="B55" s="17"/>
+      <c r="C55" s="19"/>
+      <c r="D55" s="17"/>
+      <c r="E55" s="17"/>
+      <c r="F55" s="17"/>
+      <c r="G55" s="17"/>
+      <c r="H55" s="17"/>
+      <c r="I55" s="17"/>
     </row>
     <row r="56" spans="1:9">
-      <c r="B56" s="18"/>
-      <c r="C56" s="20"/>
-      <c r="D56" s="18"/>
-      <c r="E56" s="18"/>
-      <c r="F56" s="18"/>
-      <c r="G56" s="18"/>
-      <c r="H56" s="18"/>
-      <c r="I56" s="18"/>
+      <c r="B56" s="17"/>
+      <c r="C56" s="19"/>
+      <c r="D56" s="17"/>
+      <c r="E56" s="17"/>
+      <c r="F56" s="17"/>
+      <c r="G56" s="17"/>
+      <c r="H56" s="17"/>
+      <c r="I56" s="17"/>
     </row>
     <row r="57" spans="1:9">
-      <c r="B57" s="18"/>
-      <c r="C57" s="20"/>
-      <c r="D57" s="18"/>
-      <c r="E57" s="18"/>
-      <c r="F57" s="18"/>
-      <c r="G57" s="18"/>
-      <c r="H57" s="18"/>
-      <c r="I57" s="18"/>
+      <c r="B57" s="17"/>
+      <c r="C57" s="19"/>
+      <c r="D57" s="17"/>
+      <c r="E57" s="17"/>
+      <c r="F57" s="17"/>
+      <c r="G57" s="17"/>
+      <c r="H57" s="17"/>
+      <c r="I57" s="17"/>
     </row>
     <row r="58" spans="1:9">
-      <c r="B58" s="16"/>
-      <c r="C58" s="21"/>
-      <c r="D58" s="16"/>
-      <c r="E58" s="16"/>
-      <c r="F58" s="16"/>
-      <c r="G58" s="16"/>
-      <c r="H58" s="16"/>
-      <c r="I58" s="16"/>
+      <c r="A58" s="47" t="s">
+        <v>22</v>
+      </c>
+      <c r="B58" s="47"/>
+      <c r="C58" s="47"/>
+      <c r="D58" s="47"/>
+      <c r="E58" s="47"/>
+      <c r="F58" s="47"/>
+      <c r="G58" s="47"/>
+      <c r="H58" s="47"/>
+      <c r="I58" s="47"/>
     </row>
     <row r="59" spans="1:9">
-      <c r="B59" s="16"/>
-      <c r="C59" s="21"/>
-      <c r="D59" s="16"/>
-      <c r="E59" s="16"/>
-      <c r="F59" s="16"/>
-      <c r="G59" s="16"/>
-      <c r="H59" s="16"/>
-      <c r="I59" s="16"/>
-    </row>
-    <row r="60" spans="1:9">
-      <c r="B60" s="16"/>
-      <c r="C60" s="16"/>
-      <c r="D60" s="16"/>
-      <c r="E60" s="16"/>
-      <c r="F60" s="16"/>
-      <c r="G60" s="16"/>
-      <c r="H60" s="16"/>
-      <c r="I60" s="16"/>
-    </row>
-    <row r="61" spans="1:9">
-      <c r="B61" s="16"/>
-      <c r="C61" s="16"/>
-      <c r="D61" s="16"/>
-      <c r="E61" s="16"/>
-      <c r="F61" s="16"/>
-      <c r="G61" s="16"/>
-      <c r="H61" s="16"/>
-      <c r="I61" s="16"/>
+      <c r="A59" s="33"/>
+      <c r="B59" s="33"/>
+      <c r="C59" s="33"/>
+      <c r="D59" s="33"/>
+      <c r="E59" s="33"/>
+      <c r="F59" s="33"/>
+      <c r="G59" s="33"/>
+      <c r="H59" s="33"/>
+      <c r="I59" s="33"/>
+    </row>
+    <row r="60" spans="1:9" ht="15.75">
+      <c r="A60" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="B60" s="27" t="s">
+        <v>1</v>
+      </c>
+      <c r="C60" s="27"/>
+      <c r="D60" s="14"/>
+      <c r="E60" s="27" t="s">
+        <v>2</v>
+      </c>
+      <c r="F60" s="27"/>
+      <c r="G60" s="14"/>
+      <c r="H60" s="27" t="s">
+        <v>3</v>
+      </c>
+      <c r="I60" s="27"/>
+    </row>
+    <row r="61" spans="1:9" ht="15.75">
+      <c r="A61" s="12"/>
+      <c r="B61" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="C61" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="D61" s="5"/>
+      <c r="E61" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="F61" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="G61" s="5"/>
+      <c r="H61" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="I61" s="15" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" ht="15.75">
+      <c r="A62" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="B62" s="48">
+        <f>(( 371960/96000)-B$3)*100/B$3</f>
+        <v>1.0321599304650144</v>
+      </c>
+      <c r="C62" s="49">
+        <f>371960-C$3</f>
+        <v>3800</v>
+      </c>
+      <c r="D62" s="20"/>
+      <c r="E62" s="48">
+        <f>((0/96000)-B$3)*100/B$3</f>
+        <v>-100</v>
+      </c>
+      <c r="F62" s="49">
+        <f>0-C$3</f>
+        <v>-368160</v>
+      </c>
+      <c r="G62" s="20"/>
+      <c r="H62" s="48">
+        <f>((372167/96000)-B$3)*100/B$3</f>
+        <v>1.0883854845719265</v>
+      </c>
+      <c r="I62" s="49">
+        <f>372167-C$3</f>
+        <v>4007</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" ht="15.75">
+      <c r="A63" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="B63" s="48">
+        <f>(( 382097/96000)-D$3)*100/D$3</f>
+        <v>1.7427679788684434</v>
+      </c>
+      <c r="C63" s="49">
+        <f xml:space="preserve"> 382097 -E$3</f>
+        <v>6545</v>
+      </c>
+      <c r="D63" s="20"/>
+      <c r="E63" s="48">
+        <f>((0/96000)-D$3)*100/D$3</f>
+        <v>-100</v>
+      </c>
+      <c r="F63" s="49">
+        <f>0-E$3</f>
+        <v>-375552</v>
+      </c>
+      <c r="G63" s="20"/>
+      <c r="H63" s="48">
+        <f>((382935/96000)-D$3)*100/D$3</f>
+        <v>1.9659061860940683</v>
+      </c>
+      <c r="I63" s="49">
+        <f>382935-E$3</f>
+        <v>7383</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9">
+      <c r="A64" s="3"/>
+      <c r="B64" s="16"/>
+      <c r="C64" s="18"/>
+      <c r="D64" s="17"/>
+      <c r="E64" s="17"/>
+      <c r="F64" s="18"/>
+      <c r="G64" s="16"/>
+      <c r="H64" s="17"/>
+      <c r="I64" s="17"/>
+    </row>
+    <row r="65" spans="1:9" ht="15.75">
+      <c r="A65" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="B65" s="27" t="s">
+        <v>1</v>
+      </c>
+      <c r="C65" s="27"/>
+      <c r="D65" s="14"/>
+      <c r="E65" s="27" t="s">
+        <v>2</v>
+      </c>
+      <c r="F65" s="27"/>
+      <c r="G65" s="14"/>
+      <c r="H65" s="27" t="s">
+        <v>3</v>
+      </c>
+      <c r="I65" s="27"/>
+    </row>
+    <row r="66" spans="1:9" ht="15.75">
+      <c r="A66" s="12"/>
+      <c r="B66" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="C66" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="D66" s="5"/>
+      <c r="E66" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="F66" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="G66" s="5"/>
+      <c r="H66" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="I66" s="15" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9" ht="15.75">
+      <c r="A67" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="B67" s="48">
+        <f>((536328/96000)-F$3)*100/F$3</f>
+        <v>0.40887850467290204</v>
+      </c>
+      <c r="C67" s="49">
+        <f>536328-G$3</f>
+        <v>2184</v>
+      </c>
+      <c r="D67" s="20"/>
+      <c r="E67" s="48">
+        <f>((0/96000)-F$3)*100/F$3</f>
+        <v>-100</v>
+      </c>
+      <c r="F67" s="49">
+        <f>0-G$3</f>
+        <v>-534144</v>
+      </c>
+      <c r="G67" s="20"/>
+      <c r="H67" s="48">
+        <f>((533471/96000)-F$3)*100/F$3</f>
+        <v>-0.12599598610112664</v>
+      </c>
+      <c r="I67" s="49">
+        <f>533471-G$3</f>
+        <v>-673</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9" ht="15.75">
+      <c r="A68" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="B68" s="48">
+        <f>((548254/96000)-H$3)*100/H$3</f>
+        <v>-1.2283091202582801</v>
+      </c>
+      <c r="C68" s="49">
+        <f>548254-I$3</f>
+        <v>-6818</v>
+      </c>
+      <c r="D68" s="20"/>
+      <c r="E68" s="48">
+        <f>((0/96000)-H$3)*100/H$3</f>
+        <v>-100.00000000000001</v>
+      </c>
+      <c r="F68" s="49">
+        <f>0-I$3</f>
+        <v>-555072</v>
+      </c>
+      <c r="G68" s="20"/>
+      <c r="H68" s="48">
+        <f>((563920/96000)-H$3)*100/H$3</f>
+        <v>1.5940274414850659</v>
+      </c>
+      <c r="I68" s="49">
+        <f>563920-I$3</f>
+        <v>8848</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="45">
-    <mergeCell ref="B33:C33"/>
-    <mergeCell ref="E33:F33"/>
-    <mergeCell ref="H33:I33"/>
-    <mergeCell ref="B38:C38"/>
-    <mergeCell ref="E38:F38"/>
-    <mergeCell ref="H38:I38"/>
-    <mergeCell ref="B51:C51"/>
-    <mergeCell ref="E51:F51"/>
-    <mergeCell ref="H51:I51"/>
-    <mergeCell ref="B53:C54"/>
-    <mergeCell ref="E53:F54"/>
-    <mergeCell ref="H53:I54"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="E12:F12"/>
-    <mergeCell ref="H12:I12"/>
-    <mergeCell ref="A18:I18"/>
-    <mergeCell ref="A19:I19"/>
-    <mergeCell ref="H2:I2"/>
-    <mergeCell ref="A5:I5"/>
-    <mergeCell ref="A1:A3"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="A6:I6"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="H7:I7"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="D2:E2"/>
-    <mergeCell ref="B1:E1"/>
-    <mergeCell ref="F1:I1"/>
-    <mergeCell ref="F2:G2"/>
+  <mergeCells count="53">
+    <mergeCell ref="B65:C65"/>
+    <mergeCell ref="E65:F65"/>
+    <mergeCell ref="H65:I65"/>
+    <mergeCell ref="A58:I58"/>
+    <mergeCell ref="A59:I59"/>
+    <mergeCell ref="B60:C60"/>
+    <mergeCell ref="E60:F60"/>
+    <mergeCell ref="H60:I60"/>
     <mergeCell ref="B48:C49"/>
     <mergeCell ref="E48:F49"/>
     <mergeCell ref="H48:I49"/>
@@ -1927,6 +2125,35 @@
     <mergeCell ref="H25:I25"/>
     <mergeCell ref="A44:I44"/>
     <mergeCell ref="A45:I45"/>
+    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="A5:I5"/>
+    <mergeCell ref="A1:A3"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="A6:I6"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="H7:I7"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="B1:E1"/>
+    <mergeCell ref="F1:I1"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="E12:F12"/>
+    <mergeCell ref="H12:I12"/>
+    <mergeCell ref="A18:I18"/>
+    <mergeCell ref="A19:I19"/>
+    <mergeCell ref="B51:C51"/>
+    <mergeCell ref="E51:F51"/>
+    <mergeCell ref="H51:I51"/>
+    <mergeCell ref="B53:C54"/>
+    <mergeCell ref="E53:F54"/>
+    <mergeCell ref="H53:I54"/>
+    <mergeCell ref="B33:C33"/>
+    <mergeCell ref="E33:F33"/>
+    <mergeCell ref="H33:I33"/>
+    <mergeCell ref="B38:C38"/>
+    <mergeCell ref="E38:F38"/>
+    <mergeCell ref="H38:I38"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="80" orientation="portrait" r:id="rId1"/>

</xml_diff>